<commit_message>
Add documents as PDFs
</commit_message>
<xml_diff>
--- a/docs/K-3-Teachers-Pacing-Guide.xlsx
+++ b/docs/K-3-Teachers-Pacing-Guide.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11014"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10910"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ginnykirkland/Dropbox/Voyager/Regional Marketing/South/Laura Woolf/AL LETRS/Landing Page/Resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/scottb/Projects/Voyager Sopris Learning/Microsites/Alabama LETRS/al-solutions/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F7EC691D-4B20-A647-B046-A1E6B4EF1181}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF667616-FEA9-194E-AF9F-F716EA9C1886}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="23040" windowHeight="9220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="30800" windowHeight="18060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="K-3 TCHRS" sheetId="5" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'K-3 TCHRS'!$A$1:$K$34</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'K-3 TCHRS'!$B$1:$K$34</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -724,7 +724,7 @@
   <dimension ref="B1:L38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="P28" sqref="P28"/>
+      <selection activeCell="B1" sqref="B1:K34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>

</xml_diff>